<commit_message>
Athina comments to end (some exceptions - need to re-run re-analysis tib first)
</commit_message>
<xml_diff>
--- a/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/ligthart_genome_2018.xlsx
+++ b/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/ligthart_genome_2018.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f99f7067dc2a9a5/Documents/R/Working Directory/Data_Science_MSc/Dissertation_Bayes_MR/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{34F45F51-E78E-4BCB-8BAD-F14697877A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34D6AB8C-5EDA-42B1-AF1E-95662A564AA0}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="8_{34F45F51-E78E-4BCB-8BAD-F14697877A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EB4F379-07A7-4EE4-9793-88DE0FDBF2F3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{B7A20BFC-AD9F-4C24-9E5C-C76F16BE456D}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" firstSheet="1" activeTab="5" xr2:uid="{B7A20BFC-AD9F-4C24-9E5C-C76F16BE456D}"/>
   </bookViews>
   <sheets>
     <sheet name="CRP" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Schiz" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CRP!$A$1:$C$1</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="320">
   <si>
     <t>Author</t>
   </si>
@@ -947,6 +948,75 @@
   </si>
   <si>
     <t>CRP Beta</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.010</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.011</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.012</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.013</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.014</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.015</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.016</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.017</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.018</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.019</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.020</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.021</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.022</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.023</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.024</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.025</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.026</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.027</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.028</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.029</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.030</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.031</t>
+  </si>
+  <si>
+    <t>10.1016/j.ajhg.2018.09.032</t>
   </si>
 </sst>
 </file>
@@ -1065,14 +1135,33 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1404,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82B2D2C-2E91-459F-A9A8-BB400ABE5D5D}">
   <dimension ref="A1:C143"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C98"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2074,7 +2163,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B61" t="s">
@@ -2968,7 +3057,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E54"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5388,10 +5477,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227D38A9-CD55-4855-AEA4-5F681A4CD9F1}">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E98"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6610,7 +6699,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>101</v>
       </c>
@@ -6629,7 +6718,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>92</v>
       </c>
@@ -6648,7 +6737,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -6667,7 +6756,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>52</v>
       </c>
@@ -6686,7 +6775,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>94</v>
       </c>
@@ -6705,560 +6794,1618 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="B70">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="C70">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="D70">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D70" t="e">
         <f>VLOOKUP(A70,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>1.5977051124302299</v>
-      </c>
-      <c r="E70">
+        <v>#N/A</v>
+      </c>
+      <c r="E70" t="e">
         <f>VLOOKUP($A70,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.39883720930232602</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="B71">
-        <v>2.3E-2</v>
-      </c>
-      <c r="C71">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D71">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D71" t="e">
         <f>VLOOKUP(A71,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>0.56400497515199999</v>
-      </c>
-      <c r="E71">
+        <v>#N/A</v>
+      </c>
+      <c r="E71" t="e">
         <f>VLOOKUP($A71,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.44400000000000001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B72">
-        <v>2.7E-2</v>
-      </c>
-      <c r="C72">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D72">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D72" t="e">
         <f>VLOOKUP(A72,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>0.395844662392418</v>
-      </c>
-      <c r="E72">
+        <v>#N/A</v>
+      </c>
+      <c r="E72" t="e">
         <f>VLOOKUP($A72,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.39219958601154797</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B73">
-        <v>-0.104</v>
-      </c>
-      <c r="C73">
-        <v>1.2E-2</v>
-      </c>
-      <c r="D73">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D73" t="e">
         <f>VLOOKUP(A73,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>0.275303578498655</v>
-      </c>
-      <c r="E73">
+        <v>#N/A</v>
+      </c>
+      <c r="E73" t="e">
         <f>VLOOKUP($A73,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.269058295964126</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>62</v>
-      </c>
-      <c r="B74" t="s">
-        <v>150</v>
-      </c>
-      <c r="C74" t="s">
-        <v>147</v>
-      </c>
-      <c r="D74">
+        <v>131</v>
+      </c>
+      <c r="B74">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D74" t="e">
         <f>VLOOKUP(A74,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>0.275303578498655</v>
-      </c>
-      <c r="E74">
+        <v>#N/A</v>
+      </c>
+      <c r="E74" t="e">
         <f>VLOOKUP($A74,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.269058295964126</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B75">
-        <v>-2.5999999999999999E-2</v>
-      </c>
-      <c r="C75">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D75">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D75" t="e">
         <f>VLOOKUP(A75,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>0.23764326507414599</v>
-      </c>
-      <c r="E75">
+        <v>#N/A</v>
+      </c>
+      <c r="E75" t="e">
         <f>VLOOKUP($A75,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.43520309477756303</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>71</v>
-      </c>
-      <c r="B76" t="s">
-        <v>141</v>
-      </c>
-      <c r="C76" t="s">
-        <v>142</v>
+        <v>129</v>
+      </c>
+      <c r="B76">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>195</v>
       </c>
       <c r="D76">
         <f>VLOOKUP(A76,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>0.23016734883909001</v>
+        <v>1.7445218433</v>
       </c>
       <c r="E76">
         <f>VLOOKUP($A76,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.29352315669215201</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.42962962962963003</v>
+      </c>
+      <c r="F76" t="b">
+        <f>MATCH($A76,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>69</v>
-      </c>
-      <c r="B77" t="s">
-        <v>138</v>
-      </c>
-      <c r="C77" t="s">
-        <v>134</v>
+        <v>21</v>
+      </c>
+      <c r="B77">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="C77">
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D77">
         <f>VLOOKUP(A77,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>9.7234753064520604E-2</v>
+        <v>1.5977051124302299</v>
       </c>
       <c r="E77">
         <f>VLOOKUP($A77,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.30248369640627198</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.39883720930232602</v>
+      </c>
+      <c r="F77" t="b">
+        <f>MATCH($A77,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B78">
-        <v>0.03</v>
-      </c>
-      <c r="C78">
-        <v>4.0000000000000001E-3</v>
+        <v>1.4E-2</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>194</v>
       </c>
       <c r="D78">
         <f>VLOOKUP(A78,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>8.3209924303995694E-2</v>
+        <v>1.5977051124302299</v>
       </c>
       <c r="E78">
         <f>VLOOKUP($A78,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.37324624254340699</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.39883720930232602</v>
+      </c>
+      <c r="F78" t="b">
+        <f>MATCH($A78,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>56</v>
-      </c>
-      <c r="B79" t="s">
-        <v>133</v>
-      </c>
-      <c r="C79" t="s">
-        <v>134</v>
+        <v>111</v>
+      </c>
+      <c r="B79">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C79">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D79">
         <f>VLOOKUP(A79,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>8.3209924303995694E-2</v>
+        <v>1.0566457080555001</v>
       </c>
       <c r="E79">
         <f>VLOOKUP($A79,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.37324624254340699</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.37362271245329698</v>
+      </c>
+      <c r="F79" t="b">
+        <f>MATCH($A79,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>75</v>
-      </c>
-      <c r="B80" t="s">
-        <v>149</v>
-      </c>
-      <c r="C80" t="s">
-        <v>144</v>
+        <v>125</v>
+      </c>
+      <c r="B80">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C80">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D80">
         <f>VLOOKUP(A80,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-3.7465722527858999E-2</v>
+        <v>0.90006852324166697</v>
       </c>
       <c r="E80">
         <f>VLOOKUP($A80,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>6.3627924814454895E-2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+      <c r="F80" t="b">
+        <f>MATCH($A80,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="B81">
-        <v>7.6999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="C81">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D81">
         <f>VLOOKUP(A81,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-8.30165046128611E-2</v>
+        <v>0.56400497515199999</v>
       </c>
       <c r="E81">
         <f>VLOOKUP($A81,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.14701478315319499</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="F81" t="b">
+        <f>MATCH($A81,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>28</v>
-      </c>
-      <c r="B82" t="s">
-        <v>139</v>
-      </c>
-      <c r="C82" t="s">
-        <v>134</v>
+        <v>55</v>
+      </c>
+      <c r="B82">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="D82">
         <f>VLOOKUP(A82,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-8.30165046128611E-2</v>
+        <v>0.56400497515199999</v>
       </c>
       <c r="E82">
         <f>VLOOKUP($A82,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.14701478315319499</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="F82" t="b">
+        <f>MATCH($A82,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="B83" t="s">
-        <v>135</v>
-      </c>
-      <c r="C83" t="s">
-        <v>147</v>
+        <v>185</v>
+      </c>
+      <c r="C83">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D83">
         <f>VLOOKUP(A83,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-8.7141038638266097E-2</v>
+        <v>0.48314147267521801</v>
       </c>
       <c r="E83">
         <f>VLOOKUP($A83,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.31126988535690697</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.45104123348581299</v>
+      </c>
+      <c r="F83" t="b">
+        <f>MATCH($A83,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="B84" t="s">
-        <v>140</v>
-      </c>
-      <c r="C84" t="s">
-        <v>134</v>
+        <v>192</v>
+      </c>
+      <c r="C84">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D84">
         <f>VLOOKUP(A84,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-8.9136433339484206E-2</v>
+        <v>0.42571456212602399</v>
       </c>
       <c r="E84">
         <f>VLOOKUP($A84,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.22806435561453001</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.50336338260193103</v>
+      </c>
+      <c r="F84" t="b">
+        <f>MATCH($A84,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>68</v>
-      </c>
-      <c r="B85" t="s">
-        <v>137</v>
-      </c>
-      <c r="C85" t="s">
-        <v>134</v>
+        <v>39</v>
+      </c>
+      <c r="B85">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C85">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D85">
         <f>VLOOKUP(A85,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.120735390600266</v>
+        <v>0.395844662392418</v>
       </c>
       <c r="E85">
         <f>VLOOKUP($A85,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>6.0377855598125002E-2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.39219958601154797</v>
+      </c>
+      <c r="F85" t="b">
+        <f>MATCH($A85,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="B86" t="s">
-        <v>146</v>
-      </c>
-      <c r="C86" t="s">
-        <v>134</v>
+        <v>189</v>
+      </c>
+      <c r="C86">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D86">
         <f>VLOOKUP(A86,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.14811236431004901</v>
+        <v>0.395844662392418</v>
       </c>
       <c r="E86">
         <f>VLOOKUP($A86,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>7.8788984132774006E-2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.39219958601154797</v>
+      </c>
+      <c r="F86" t="b">
+        <f>MATCH($A86,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>73</v>
-      </c>
-      <c r="B87" t="s">
-        <v>176</v>
-      </c>
-      <c r="C87" t="s">
-        <v>134</v>
+        <v>62</v>
+      </c>
+      <c r="B87">
+        <v>-0.104</v>
+      </c>
+      <c r="C87">
+        <v>1.2E-2</v>
       </c>
       <c r="D87">
         <f>VLOOKUP(A87,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.14811236431004901</v>
+        <v>0.275303578498655</v>
       </c>
       <c r="E87">
         <f>VLOOKUP($A87,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>7.8788984132774006E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.269058295964126</v>
+      </c>
+      <c r="F87" t="b">
+        <f>MATCH($A87,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B88" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="C88" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="D88">
         <f>VLOOKUP(A88,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.20979362816125499</v>
+        <v>0.275303578498655</v>
       </c>
       <c r="E88">
         <f>VLOOKUP($A88,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.105383163602571</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.269058295964126</v>
+      </c>
+      <c r="F88" t="b">
+        <f>MATCH($A88,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>67</v>
-      </c>
-      <c r="B89" t="s">
-        <v>136</v>
-      </c>
-      <c r="C89" t="s">
-        <v>134</v>
+        <v>37</v>
+      </c>
+      <c r="B89">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="C89">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D89">
         <f>VLOOKUP(A89,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.29361608436110997</v>
+        <v>0.23764326507414599</v>
       </c>
       <c r="E89">
         <f>VLOOKUP($A89,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.12340177561443801</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.43520309477756303</v>
+      </c>
+      <c r="F89" t="b">
+        <f>MATCH($A89,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>22</v>
-      </c>
-      <c r="B90">
-        <v>3.5000000000000003E-2</v>
+        <v>37</v>
+      </c>
+      <c r="B90" t="s">
+        <v>186</v>
       </c>
       <c r="C90">
-        <v>5.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D90">
         <f>VLOOKUP(A90,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.32043034098407203</v>
+        <v>0.23764326507414599</v>
       </c>
       <c r="E90">
         <f>VLOOKUP($A90,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.41966823078448201</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.43520309477756303</v>
+      </c>
+      <c r="F90" t="b">
+        <f>MATCH($A90,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B91" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C91" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="D91">
         <f>VLOOKUP(A91,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.32043034098407203</v>
+        <v>0.23016734883909001</v>
       </c>
       <c r="E91">
         <f>VLOOKUP($A91,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.41966823078448201</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.29352315669215201</v>
+      </c>
+      <c r="F91" t="b">
+        <f>MATCH($A91,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>53</v>
-      </c>
-      <c r="B92">
-        <v>-3.5999999999999997E-2</v>
+        <v>128</v>
+      </c>
+      <c r="B92" t="s">
+        <v>189</v>
       </c>
       <c r="C92">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D92">
         <f>VLOOKUP(A92,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.41431075563352499</v>
+        <v>0.20152708546981199</v>
       </c>
       <c r="E92">
         <f>VLOOKUP($A92,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.309998872731372</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.39555539573519399</v>
+      </c>
+      <c r="F92" t="b">
+        <f>MATCH($A92,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="B93" t="s">
-        <v>148</v>
-      </c>
-      <c r="C93" t="s">
-        <v>134</v>
+        <v>186</v>
+      </c>
+      <c r="C93">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D93">
         <f>VLOOKUP(A93,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.42470121872245797</v>
+        <v>0.19650105360627501</v>
       </c>
       <c r="E93">
         <f>VLOOKUP($A93,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.43662825955124301</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.433282516248094</v>
+      </c>
+      <c r="F93" t="b">
+        <f>MATCH($A93,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="B94">
-        <v>-9.6000000000000002E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="C94">
-        <v>1.6E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D94">
         <f>VLOOKUP(A94,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.43834270734766401</v>
+        <v>0.17582189386248501</v>
       </c>
       <c r="E94">
         <f>VLOOKUP($A94,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.38691588785046699</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.48155437376994298</v>
+      </c>
+      <c r="F94" t="b">
+        <f>MATCH($A94,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>49</v>
-      </c>
-      <c r="B95">
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="C95">
-        <v>4.0000000000000001E-3</v>
+        <v>69</v>
+      </c>
+      <c r="B95" t="s">
+        <v>138</v>
+      </c>
+      <c r="C95" t="s">
+        <v>134</v>
       </c>
       <c r="D95">
         <f>VLOOKUP(A95,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.62889153521509</v>
+        <v>9.7234753064520604E-2</v>
       </c>
       <c r="E95">
         <f>VLOOKUP($A95,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.50662686027050297</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.30248369640627198</v>
+      </c>
+      <c r="F95" t="b">
+        <f>MATCH($A95,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>20</v>
-      </c>
-      <c r="B96" t="s">
-        <v>145</v>
-      </c>
-      <c r="C96" t="s">
-        <v>134</v>
+        <v>56</v>
+      </c>
+      <c r="B96">
+        <v>0.03</v>
+      </c>
+      <c r="C96">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D96">
         <f>VLOOKUP(A96,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.73694337285361899</v>
+        <v>8.3209924303995694E-2</v>
       </c>
       <c r="E96">
         <f>VLOOKUP($A96,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.32188195656097701</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.37324624254340699</v>
+      </c>
+      <c r="F96" t="b">
+        <f>MATCH($A96,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>47</v>
-      </c>
-      <c r="B97">
-        <v>2.3E-2</v>
-      </c>
-      <c r="C97">
-        <v>4.0000000000000001E-3</v>
+        <v>56</v>
+      </c>
+      <c r="B97" t="s">
+        <v>133</v>
+      </c>
+      <c r="C97" t="s">
+        <v>134</v>
       </c>
       <c r="D97">
         <f>VLOOKUP(A97,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-0.84798952666127003</v>
+        <v>8.3209924303995694E-2</v>
       </c>
       <c r="E97">
         <f>VLOOKUP($A97,Schiz!$A$2:$E$54, 3,FALSE)</f>
-        <v>0.431699044094974</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.37324624254340699</v>
+      </c>
+      <c r="F97" t="b">
+        <f>MATCH($A97,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="B98" t="s">
-        <v>143</v>
-      </c>
-      <c r="C98" t="s">
-        <v>144</v>
+        <v>185</v>
+      </c>
+      <c r="C98">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D98">
         <f>VLOOKUP(A98,Schiz!$A$2:$E$54, 2,FALSE)</f>
-        <v>-1.2550855746723999</v>
+        <v>6.7778038905043497E-2</v>
       </c>
       <c r="E98">
         <f>VLOOKUP($A98,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.40709508578074999</v>
+      </c>
+      <c r="F98" t="b">
+        <f>MATCH($A98,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>16</v>
+      </c>
+      <c r="B99" t="s">
+        <v>193</v>
+      </c>
+      <c r="C99">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D99">
+        <f>VLOOKUP(A99,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-1.6241641763504899E-2</v>
+      </c>
+      <c r="E99">
+        <f>VLOOKUP($A99,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.37096206439035001</v>
+      </c>
+      <c r="F99" t="b">
+        <f>MATCH($A99,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>75</v>
+      </c>
+      <c r="B100" t="s">
+        <v>149</v>
+      </c>
+      <c r="C100" t="s">
+        <v>144</v>
+      </c>
+      <c r="D100">
+        <f>VLOOKUP(A100,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-3.7465722527858999E-2</v>
+      </c>
+      <c r="E100">
+        <f>VLOOKUP($A100,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>6.3627924814454895E-2</v>
+      </c>
+      <c r="F100" t="b">
+        <f>MATCH($A100,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101" t="s">
+        <v>185</v>
+      </c>
+      <c r="C101">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D101">
+        <f>VLOOKUP(A101,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-6.3778933912280095E-2</v>
+      </c>
+      <c r="E101">
+        <f>VLOOKUP($A101,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.430938168353178</v>
+      </c>
+      <c r="F101" t="b">
+        <f>MATCH($A101,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>28</v>
+      </c>
+      <c r="B102">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C102">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D102">
+        <f>VLOOKUP(A102,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-8.30165046128611E-2</v>
+      </c>
+      <c r="E102">
+        <f>VLOOKUP($A102,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.14701478315319499</v>
+      </c>
+      <c r="F102" t="b">
+        <f>MATCH($A102,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>28</v>
+      </c>
+      <c r="B103" t="s">
+        <v>139</v>
+      </c>
+      <c r="C103" t="s">
+        <v>134</v>
+      </c>
+      <c r="D103">
+        <f>VLOOKUP(A103,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-8.30165046128611E-2</v>
+      </c>
+      <c r="E103">
+        <f>VLOOKUP($A103,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.14701478315319499</v>
+      </c>
+      <c r="F103" t="b">
+        <f>MATCH($A103,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>19</v>
+      </c>
+      <c r="B104" t="s">
+        <v>135</v>
+      </c>
+      <c r="C104" t="s">
+        <v>147</v>
+      </c>
+      <c r="D104">
+        <f>VLOOKUP(A104,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-8.7141038638266097E-2</v>
+      </c>
+      <c r="E104">
+        <f>VLOOKUP($A104,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.31126988535690697</v>
+      </c>
+      <c r="F104" t="b">
+        <f>MATCH($A104,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>70</v>
+      </c>
+      <c r="B105" t="s">
+        <v>140</v>
+      </c>
+      <c r="C105" t="s">
+        <v>134</v>
+      </c>
+      <c r="D105">
+        <f>VLOOKUP(A105,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-8.9136433339484206E-2</v>
+      </c>
+      <c r="E105">
+        <f>VLOOKUP($A105,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.22806435561453001</v>
+      </c>
+      <c r="F105" t="b">
+        <f>MATCH($A105,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>68</v>
+      </c>
+      <c r="B106" t="s">
+        <v>137</v>
+      </c>
+      <c r="C106" t="s">
+        <v>134</v>
+      </c>
+      <c r="D106">
+        <f>VLOOKUP(A106,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.120735390600266</v>
+      </c>
+      <c r="E106">
+        <f>VLOOKUP($A106,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>6.0377855598125002E-2</v>
+      </c>
+      <c r="F106" t="b">
+        <f>MATCH($A106,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>116</v>
+      </c>
+      <c r="B107" t="s">
+        <v>191</v>
+      </c>
+      <c r="C107">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D107">
+        <f>VLOOKUP(A107,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.120997261509139</v>
+      </c>
+      <c r="E107">
+        <f>VLOOKUP($A107,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.52872752908001397</v>
+      </c>
+      <c r="F107" t="b">
+        <f>MATCH($A107,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>73</v>
+      </c>
+      <c r="B108" t="s">
+        <v>146</v>
+      </c>
+      <c r="C108" t="s">
+        <v>134</v>
+      </c>
+      <c r="D108">
+        <f>VLOOKUP(A108,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.14811236431004901</v>
+      </c>
+      <c r="E108">
+        <f>VLOOKUP($A108,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>7.8788984132774006E-2</v>
+      </c>
+      <c r="F108" t="b">
+        <f>MATCH($A108,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>73</v>
+      </c>
+      <c r="B109" t="s">
+        <v>176</v>
+      </c>
+      <c r="C109" t="s">
+        <v>134</v>
+      </c>
+      <c r="D109">
+        <f>VLOOKUP(A109,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.14811236431004901</v>
+      </c>
+      <c r="E109">
+        <f>VLOOKUP($A109,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>7.8788984132774006E-2</v>
+      </c>
+      <c r="F109" t="b">
+        <f>MATCH($A109,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="C110">
+        <v>0.01</v>
+      </c>
+      <c r="D110">
+        <f>VLOOKUP(A110,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.18530099117117799</v>
+      </c>
+      <c r="E110">
+        <f>VLOOKUP($A110,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.50028793550244699</v>
+      </c>
+      <c r="F110" t="b">
+        <f>MATCH($A110,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>122</v>
+      </c>
+      <c r="B111">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C111">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D111">
+        <f>VLOOKUP(A111,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.185692452647822</v>
+      </c>
+      <c r="E111">
+        <f>VLOOKUP($A111,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.32128750810587797</v>
+      </c>
+      <c r="F111" t="b">
+        <f>MATCH($A111,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>66</v>
+      </c>
+      <c r="B112" t="s">
+        <v>135</v>
+      </c>
+      <c r="C112" t="s">
+        <v>134</v>
+      </c>
+      <c r="D112">
+        <f>VLOOKUP(A112,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.20979362816125499</v>
+      </c>
+      <c r="E112">
+        <f>VLOOKUP($A112,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.105383163602571</v>
+      </c>
+      <c r="F112" t="b">
+        <f>MATCH($A112,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>127</v>
+      </c>
+      <c r="B113">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="C113">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D113">
+        <f>VLOOKUP(A113,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.22385287731784101</v>
+      </c>
+      <c r="E113">
+        <f>VLOOKUP($A113,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.28436902708498402</v>
+      </c>
+      <c r="F113" t="b">
+        <f>MATCH($A113,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>120</v>
+      </c>
+      <c r="B114" t="s">
+        <v>189</v>
+      </c>
+      <c r="C114">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D114">
+        <f>VLOOKUP(A114,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.28673559390332198</v>
+      </c>
+      <c r="E114">
+        <f>VLOOKUP($A114,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.38341634715304401</v>
+      </c>
+      <c r="F114" t="b">
+        <f>MATCH($A114,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>67</v>
+      </c>
+      <c r="B115" t="s">
+        <v>136</v>
+      </c>
+      <c r="C115" t="s">
+        <v>134</v>
+      </c>
+      <c r="D115">
+        <f>VLOOKUP(A115,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.29361608436110997</v>
+      </c>
+      <c r="E115">
+        <f>VLOOKUP($A115,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.12340177561443801</v>
+      </c>
+      <c r="F115" t="b">
+        <f>MATCH($A115,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>112</v>
+      </c>
+      <c r="B116" t="s">
+        <v>187</v>
+      </c>
+      <c r="C116">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D116">
+        <f>VLOOKUP(A116,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.298055121920277</v>
+      </c>
+      <c r="E116">
+        <f>VLOOKUP($A116,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.48237151376951398</v>
+      </c>
+      <c r="F116" t="b">
+        <f>MATCH($A116,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>22</v>
+      </c>
+      <c r="B117">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C117">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D117">
+        <f>VLOOKUP(A117,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.32043034098407203</v>
+      </c>
+      <c r="E117">
+        <f>VLOOKUP($A117,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.41966823078448201</v>
+      </c>
+      <c r="F117" t="b">
+        <f>MATCH($A117,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>22</v>
+      </c>
+      <c r="B118" t="s">
+        <v>133</v>
+      </c>
+      <c r="C118" t="s">
+        <v>134</v>
+      </c>
+      <c r="D118">
+        <f>VLOOKUP(A118,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.32043034098407203</v>
+      </c>
+      <c r="E118">
+        <f>VLOOKUP($A118,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.41966823078448201</v>
+      </c>
+      <c r="F118" t="b">
+        <f>MATCH($A118,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>124</v>
+      </c>
+      <c r="B119" t="s">
+        <v>190</v>
+      </c>
+      <c r="C119">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D119">
+        <f>VLOOKUP(A119,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.35304644548957498</v>
+      </c>
+      <c r="E119">
+        <f>VLOOKUP($A119,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.40752465160280898</v>
+      </c>
+      <c r="F119" t="b">
+        <f>MATCH($A119,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>107</v>
+      </c>
+      <c r="B120">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C120">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D120">
+        <f>VLOOKUP(A120,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.36616018228963698</v>
+      </c>
+      <c r="E120">
+        <f>VLOOKUP($A120,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.457707799340901</v>
+      </c>
+      <c r="F120" t="b">
+        <f>MATCH($A120,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>53</v>
+      </c>
+      <c r="B121">
+        <v>-3.5999999999999997E-2</v>
+      </c>
+      <c r="C121">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D121">
+        <f>VLOOKUP(A121,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.41431075563352499</v>
+      </c>
+      <c r="E121">
+        <f>VLOOKUP($A121,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.309998872731372</v>
+      </c>
+      <c r="F121" t="b">
+        <f>MATCH($A121,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>53</v>
+      </c>
+      <c r="B122">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C122">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D122">
+        <f>VLOOKUP(A122,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.41431075563352499</v>
+      </c>
+      <c r="E122">
+        <f>VLOOKUP($A122,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.309998872731372</v>
+      </c>
+      <c r="F122" t="b">
+        <f>MATCH($A122,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>74</v>
+      </c>
+      <c r="B123" t="s">
+        <v>148</v>
+      </c>
+      <c r="C123" t="s">
+        <v>134</v>
+      </c>
+      <c r="D123">
+        <f>VLOOKUP(A123,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.42470121872245797</v>
+      </c>
+      <c r="E123">
+        <f>VLOOKUP($A123,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.43662825955124301</v>
+      </c>
+      <c r="F123" t="b">
+        <f>MATCH($A123,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>106</v>
+      </c>
+      <c r="B124">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C124">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D124">
+        <f>VLOOKUP(A124,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.43493149949916099</v>
+      </c>
+      <c r="E124">
+        <f>VLOOKUP($A124,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.48497484476272501</v>
+      </c>
+      <c r="F124" t="b">
+        <f>MATCH($A124,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>54</v>
+      </c>
+      <c r="B125">
+        <v>-9.6000000000000002E-2</v>
+      </c>
+      <c r="C125">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D125">
+        <f>VLOOKUP(A125,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.43834270734766401</v>
+      </c>
+      <c r="E125">
+        <f>VLOOKUP($A125,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.38691588785046699</v>
+      </c>
+      <c r="F125" t="b">
+        <f>MATCH($A125,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>54</v>
+      </c>
+      <c r="B126">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C126" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D126">
+        <f>VLOOKUP(A126,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.43834270734766401</v>
+      </c>
+      <c r="E126">
+        <f>VLOOKUP($A126,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.38691588785046699</v>
+      </c>
+      <c r="F126" t="b">
+        <f>MATCH($A126,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>114</v>
+      </c>
+      <c r="B127">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C127">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D127">
+        <f>VLOOKUP(A127,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.46565820135735098</v>
+      </c>
+      <c r="E127">
+        <f>VLOOKUP($A127,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.51735490546514895</v>
+      </c>
+      <c r="F127" t="b">
+        <f>MATCH($A127,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>121</v>
+      </c>
+      <c r="B128" t="s">
+        <v>192</v>
+      </c>
+      <c r="C128">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D128">
+        <f>VLOOKUP(A128,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.50507817642654196</v>
+      </c>
+      <c r="E128">
+        <f>VLOOKUP($A128,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.49167756777482102</v>
+      </c>
+      <c r="F128" t="b">
+        <f>MATCH($A128,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>113</v>
+      </c>
+      <c r="B129" t="s">
+        <v>188</v>
+      </c>
+      <c r="C129">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D129">
+        <f>VLOOKUP(A129,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.54393212711267602</v>
+      </c>
+      <c r="E129">
+        <f>VLOOKUP($A129,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.44209702660406902</v>
+      </c>
+      <c r="F129" t="b">
+        <f>MATCH($A129,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>49</v>
+      </c>
+      <c r="B130">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="C130">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D130">
+        <f>VLOOKUP(A130,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.62889153521509</v>
+      </c>
+      <c r="E130">
+        <f>VLOOKUP($A130,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.50662686027050297</v>
+      </c>
+      <c r="F130" t="b">
+        <f>MATCH($A130,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>49</v>
+      </c>
+      <c r="B131" t="s">
+        <v>192</v>
+      </c>
+      <c r="C131">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D131">
+        <f>VLOOKUP(A131,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.62889153521509</v>
+      </c>
+      <c r="E131">
+        <f>VLOOKUP($A131,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.50662686027050297</v>
+      </c>
+      <c r="F131" t="b">
+        <f>MATCH($A131,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>117</v>
+      </c>
+      <c r="B132">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C132">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D132">
+        <f>VLOOKUP(A132,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.68361041975036396</v>
+      </c>
+      <c r="E132">
+        <f>VLOOKUP($A132,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.48074802628677299</v>
+      </c>
+      <c r="F132" t="b">
+        <f>MATCH($A132,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>20</v>
+      </c>
+      <c r="B133" t="s">
+        <v>145</v>
+      </c>
+      <c r="C133" t="s">
+        <v>134</v>
+      </c>
+      <c r="D133">
+        <f>VLOOKUP(A133,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.73694337285361899</v>
+      </c>
+      <c r="E133">
+        <f>VLOOKUP($A133,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.32188195656097701</v>
+      </c>
+      <c r="F133" t="b">
+        <f>MATCH($A133,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>47</v>
+      </c>
+      <c r="B134">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C134">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D134">
+        <f>VLOOKUP(A134,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.84798952666127003</v>
+      </c>
+      <c r="E134">
+        <f>VLOOKUP($A134,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.431699044094974</v>
+      </c>
+      <c r="F134" t="b">
+        <f>MATCH($A134,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>47</v>
+      </c>
+      <c r="B135" t="s">
+        <v>188</v>
+      </c>
+      <c r="C135">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D135">
+        <f>VLOOKUP(A135,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.84798952666127003</v>
+      </c>
+      <c r="E135">
+        <f>VLOOKUP($A135,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.431699044094974</v>
+      </c>
+      <c r="F135" t="b">
+        <f>MATCH($A135,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>123</v>
+      </c>
+      <c r="B136">
+        <v>0.02</v>
+      </c>
+      <c r="C136">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D136">
+        <f>VLOOKUP(A136,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.85433760262868597</v>
+      </c>
+      <c r="E136">
+        <f>VLOOKUP($A136,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.53973013493253397</v>
+      </c>
+      <c r="F136" t="b">
+        <f>MATCH($A136,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>126</v>
+      </c>
+      <c r="B137" t="s">
+        <v>187</v>
+      </c>
+      <c r="C137">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D137">
+        <f>VLOOKUP(A137,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-1.0825650582392301</v>
+      </c>
+      <c r="E137">
+        <f>VLOOKUP($A137,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.485788554139856</v>
+      </c>
+      <c r="F137" t="b">
+        <f>MATCH($A137,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>72</v>
+      </c>
+      <c r="B138" t="s">
+        <v>143</v>
+      </c>
+      <c r="C138" t="s">
+        <v>144</v>
+      </c>
+      <c r="D138">
+        <f>VLOOKUP(A138,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-1.2550855746723999</v>
+      </c>
+      <c r="E138">
+        <f>VLOOKUP($A138,Schiz!$A$2:$E$54, 3,FALSE)</f>
         <v>0.28880866425992802</v>
+      </c>
+      <c r="F138" t="b">
+        <f>MATCH($A138,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>109</v>
+      </c>
+      <c r="B139">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C139">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D139">
+        <f>VLOOKUP(A139,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-1.3374852552877901</v>
+      </c>
+      <c r="E139">
+        <f>VLOOKUP($A139,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.46993613688396202</v>
+      </c>
+      <c r="F139" t="b">
+        <f>MATCH($A139,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>115</v>
+      </c>
+      <c r="B140" t="s">
+        <v>190</v>
+      </c>
+      <c r="C140">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D140">
+        <f>VLOOKUP(A140,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-1.38337156657076</v>
+      </c>
+      <c r="E140">
+        <f>VLOOKUP($A140,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.39098520895577399</v>
+      </c>
+      <c r="F140" t="b">
+        <f>MATCH($A140,Schiz!$A$3:$A$54,0) &gt;0</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{227D38A9-CD55-4855-AEA4-5F681A4CD9F1}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E98">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E140">
       <sortCondition descending="1" ref="D1"/>
     </sortState>
   </autoFilter>
@@ -7267,11 +8414,1034 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43620535-5871-407B-AC02-542967AF396D}">
+  <dimension ref="A1:E53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2">
+        <f>VLOOKUP(A2,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>1.7445218433</v>
+      </c>
+      <c r="E2">
+        <f>VLOOKUP($A2,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.42962962962963003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <f>VLOOKUP(A3,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>1.5977051124302299</v>
+      </c>
+      <c r="E3">
+        <f>VLOOKUP($A3,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.39883720930232602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D4">
+        <f>VLOOKUP(A4,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>1.0566457080555001</v>
+      </c>
+      <c r="E4">
+        <f>VLOOKUP($A4,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.37362271245329698</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D5">
+        <f>VLOOKUP(A5,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>0.90006852324166697</v>
+      </c>
+      <c r="E5">
+        <f>VLOOKUP($A5,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D6">
+        <f>VLOOKUP(A6,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>0.56400497515199999</v>
+      </c>
+      <c r="E6">
+        <f>VLOOKUP($A6,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D7">
+        <f>VLOOKUP(A7,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>0.48314147267521801</v>
+      </c>
+      <c r="E7">
+        <f>VLOOKUP($A7,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.45104123348581299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D8">
+        <f>VLOOKUP(A8,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>0.42571456212602399</v>
+      </c>
+      <c r="E8">
+        <f>VLOOKUP($A8,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.50336338260193103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D9">
+        <f>VLOOKUP(A9,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>0.395844662392418</v>
+      </c>
+      <c r="E9">
+        <f>VLOOKUP($A9,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.39219958601154797</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10">
+        <v>-0.104</v>
+      </c>
+      <c r="C10">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D10">
+        <f>VLOOKUP(A10,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>0.275303578498655</v>
+      </c>
+      <c r="E10">
+        <f>VLOOKUP($A10,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.269058295964126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="C11">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D11">
+        <f>VLOOKUP(A11,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>0.23764326507414599</v>
+      </c>
+      <c r="E11">
+        <f>VLOOKUP($A11,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.43520309477756303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12">
+        <f>VLOOKUP(A12,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>0.23016734883909001</v>
+      </c>
+      <c r="E12">
+        <f>VLOOKUP($A12,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.29352315669215201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D13">
+        <f>VLOOKUP(A13,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>0.20152708546981199</v>
+      </c>
+      <c r="E13">
+        <f>VLOOKUP($A13,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.39555539573519399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D14">
+        <f>VLOOKUP(A14,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>0.19650105360627501</v>
+      </c>
+      <c r="E14">
+        <f>VLOOKUP($A14,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.433282516248094</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D15">
+        <f>VLOOKUP(A15,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>0.17582189386248501</v>
+      </c>
+      <c r="E15">
+        <f>VLOOKUP($A15,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.48155437376994298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16">
+        <f>VLOOKUP(A16,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>9.7234753064520604E-2</v>
+      </c>
+      <c r="E16">
+        <f>VLOOKUP($A16,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.30248369640627198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17">
+        <v>0.03</v>
+      </c>
+      <c r="C17">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D17">
+        <f>VLOOKUP(A17,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>8.3209924303995694E-2</v>
+      </c>
+      <c r="E17">
+        <f>VLOOKUP($A17,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.37324624254340699</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>185</v>
+      </c>
+      <c r="C18">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D18">
+        <f>VLOOKUP(A18,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>6.7778038905043497E-2</v>
+      </c>
+      <c r="E18">
+        <f>VLOOKUP($A18,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.40709508578074999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D19">
+        <f>VLOOKUP(A19,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-1.6241641763504899E-2</v>
+      </c>
+      <c r="E19">
+        <f>VLOOKUP($A19,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.37096206439035001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20">
+        <f>VLOOKUP(A20,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-3.7465722527858999E-2</v>
+      </c>
+      <c r="E20">
+        <f>VLOOKUP($A20,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>6.3627924814454895E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D21">
+        <f>VLOOKUP(A21,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-6.3778933912280095E-2</v>
+      </c>
+      <c r="E21">
+        <f>VLOOKUP($A21,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.430938168353178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C22">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D22">
+        <f>VLOOKUP(A22,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-8.30165046128611E-2</v>
+      </c>
+      <c r="E22">
+        <f>VLOOKUP($A22,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.14701478315319499</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23">
+        <f>VLOOKUP(A23,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-8.7141038638266097E-2</v>
+      </c>
+      <c r="E23">
+        <f>VLOOKUP($A23,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.31126988535690697</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24">
+        <f>VLOOKUP(A24,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-8.9136433339484206E-2</v>
+      </c>
+      <c r="E24">
+        <f>VLOOKUP($A24,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.22806435561453001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25">
+        <f>VLOOKUP(A25,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.120735390600266</v>
+      </c>
+      <c r="E25">
+        <f>VLOOKUP($A25,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>6.0377855598125002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D26">
+        <f>VLOOKUP(A26,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.120997261509139</v>
+      </c>
+      <c r="E26">
+        <f>VLOOKUP($A26,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.52872752908001397</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27">
+        <f>VLOOKUP(A27,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.14811236431004901</v>
+      </c>
+      <c r="E27">
+        <f>VLOOKUP($A27,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>7.8788984132774006E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="C28">
+        <v>0.01</v>
+      </c>
+      <c r="D28">
+        <f>VLOOKUP(A28,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.18530099117117799</v>
+      </c>
+      <c r="E28">
+        <f>VLOOKUP($A28,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.50028793550244699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C29">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D29">
+        <f>VLOOKUP(A29,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.185692452647822</v>
+      </c>
+      <c r="E29">
+        <f>VLOOKUP($A29,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.32128750810587797</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30">
+        <f>VLOOKUP(A30,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.20979362816125499</v>
+      </c>
+      <c r="E30">
+        <f>VLOOKUP($A30,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.105383163602571</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="C31">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D31">
+        <f>VLOOKUP(A31,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.22385287731784101</v>
+      </c>
+      <c r="E31">
+        <f>VLOOKUP($A31,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.28436902708498402</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D32">
+        <f>VLOOKUP(A32,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.28673559390332198</v>
+      </c>
+      <c r="E32">
+        <f>VLOOKUP($A32,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.38341634715304401</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33">
+        <f>VLOOKUP(A33,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.29361608436110997</v>
+      </c>
+      <c r="E33">
+        <f>VLOOKUP($A33,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.12340177561443801</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C34">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D34">
+        <f>VLOOKUP(A34,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.298055121920277</v>
+      </c>
+      <c r="E34">
+        <f>VLOOKUP($A34,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.48237151376951398</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C35">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D35">
+        <f>VLOOKUP(A35,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.32043034098407203</v>
+      </c>
+      <c r="E35">
+        <f>VLOOKUP($A35,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.41966823078448201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" t="s">
+        <v>190</v>
+      </c>
+      <c r="C36">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D36">
+        <f>VLOOKUP(A36,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.35304644548957498</v>
+      </c>
+      <c r="E36">
+        <f>VLOOKUP($A36,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.40752465160280898</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C37">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D37">
+        <f>VLOOKUP(A37,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.36616018228963698</v>
+      </c>
+      <c r="E37">
+        <f>VLOOKUP($A37,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.457707799340901</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C38">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D38">
+        <f>VLOOKUP(A38,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.41431075563352499</v>
+      </c>
+      <c r="E38">
+        <f>VLOOKUP($A38,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.309998872731372</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39">
+        <f>VLOOKUP(A39,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.42470121872245797</v>
+      </c>
+      <c r="E39">
+        <f>VLOOKUP($A39,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.43662825955124301</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C40">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D40">
+        <f>VLOOKUP(A40,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.43493149949916099</v>
+      </c>
+      <c r="E40">
+        <f>VLOOKUP($A40,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.48497484476272501</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41">
+        <v>-9.6000000000000002E-2</v>
+      </c>
+      <c r="C41">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D41">
+        <f>VLOOKUP(A41,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.43834270734766401</v>
+      </c>
+      <c r="E41">
+        <f>VLOOKUP($A41,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.38691588785046699</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C42">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D42">
+        <f>VLOOKUP(A42,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.46565820135735098</v>
+      </c>
+      <c r="E42">
+        <f>VLOOKUP($A42,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.51735490546514895</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" t="s">
+        <v>192</v>
+      </c>
+      <c r="C43">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D43">
+        <f>VLOOKUP(A43,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.50507817642654196</v>
+      </c>
+      <c r="E43">
+        <f>VLOOKUP($A43,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.49167756777482102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D44">
+        <f>VLOOKUP(A44,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.54393212711267602</v>
+      </c>
+      <c r="E44">
+        <f>VLOOKUP($A44,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.44209702660406902</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="C45">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D45">
+        <f>VLOOKUP(A45,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.62889153521509</v>
+      </c>
+      <c r="E45">
+        <f>VLOOKUP($A45,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.50662686027050297</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C46">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D46">
+        <f>VLOOKUP(A46,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.68361041975036396</v>
+      </c>
+      <c r="E46">
+        <f>VLOOKUP($A46,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.48074802628677299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" t="s">
+        <v>134</v>
+      </c>
+      <c r="D47">
+        <f>VLOOKUP(A47,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.73694337285361899</v>
+      </c>
+      <c r="E47">
+        <f>VLOOKUP($A47,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.32188195656097701</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D48">
+        <f>VLOOKUP(A48,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.84798952666127003</v>
+      </c>
+      <c r="E48">
+        <f>VLOOKUP($A48,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.431699044094974</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49">
+        <v>0.02</v>
+      </c>
+      <c r="C49">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D49">
+        <f>VLOOKUP(A49,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-0.85433760262868597</v>
+      </c>
+      <c r="E49">
+        <f>VLOOKUP($A49,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.53973013493253397</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B50" t="s">
+        <v>187</v>
+      </c>
+      <c r="C50">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D50">
+        <f>VLOOKUP(A50,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-1.0825650582392301</v>
+      </c>
+      <c r="E50">
+        <f>VLOOKUP($A50,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.485788554139856</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B51" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51">
+        <f>VLOOKUP(A51,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-1.2550855746723999</v>
+      </c>
+      <c r="E51">
+        <f>VLOOKUP($A51,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.28880866425992802</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C52">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D52">
+        <f>VLOOKUP(A52,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-1.3374852552877901</v>
+      </c>
+      <c r="E52">
+        <f>VLOOKUP($A52,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.46993613688396202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" t="s">
+        <v>190</v>
+      </c>
+      <c r="C53">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D53">
+        <f>VLOOKUP(A53,Schiz!$A$2:$E$54, 2,FALSE)</f>
+        <v>-1.38337156657076</v>
+      </c>
+      <c r="E53">
+        <f>VLOOKUP($A53,Schiz!$A$2:$E$54, 3,FALSE)</f>
+        <v>0.39098520895577399</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12442AF0-49F8-4410-8BEE-3F58D7D3AEC7}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G30"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7328,22 +9498,22 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
       </c>
       <c r="H2">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="I2">
-        <v>1.2999999999999999E-2</v>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>195</v>
       </c>
       <c r="J2">
-        <v>1.5977051124302299</v>
+        <v>1.7445218433</v>
       </c>
       <c r="K2">
-        <v>0.39883720930232602</v>
+        <v>0.42962962962963003</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -7363,22 +9533,22 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
         <v>17</v>
       </c>
       <c r="H3">
-        <v>2.3E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="I3">
-        <v>4.0000000000000001E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="J3">
-        <v>0.56400497515199999</v>
+        <v>1.5977051124302299</v>
       </c>
       <c r="K3">
-        <v>0.44400000000000001</v>
+        <v>0.39883720930232602</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -7398,22 +9568,22 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>111</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
       </c>
       <c r="H4">
-        <v>2.7E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="I4">
-        <v>4.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="J4">
-        <v>0.395844662392418</v>
+        <v>1.0566457080555001</v>
       </c>
       <c r="K4">
-        <v>0.39219958601154797</v>
+        <v>0.37362271245329698</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -7433,22 +9603,22 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
       </c>
       <c r="H5">
-        <v>-0.104</v>
+        <v>2.4E-2</v>
       </c>
       <c r="I5">
-        <v>1.2E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J5">
-        <v>0.275303578498655</v>
+        <v>0.90006852324166697</v>
       </c>
       <c r="K5">
-        <v>0.269058295964126</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -7468,22 +9638,22 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
       </c>
-      <c r="H6" t="s">
-        <v>150</v>
-      </c>
-      <c r="I6" t="s">
-        <v>147</v>
+      <c r="H6">
+        <v>2.3E-2</v>
+      </c>
+      <c r="I6">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J6">
-        <v>0.275303578498655</v>
+        <v>0.56400497515199999</v>
       </c>
       <c r="K6">
-        <v>0.269058295964126</v>
+        <v>0.44400000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -7503,22 +9673,22 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="H7">
-        <v>-2.5999999999999999E-2</v>
+      <c r="H7" t="s">
+        <v>185</v>
       </c>
       <c r="I7">
-        <v>4.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="J7">
-        <v>0.23764326507414599</v>
+        <v>0.48314147267521801</v>
       </c>
       <c r="K7">
-        <v>0.43520309477756303</v>
+        <v>0.45104123348581299</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -7538,22 +9708,22 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>141</v>
-      </c>
-      <c r="I8" t="s">
-        <v>142</v>
+        <v>192</v>
+      </c>
+      <c r="I8">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J8">
-        <v>0.23016734883909001</v>
+        <v>0.42571456212602399</v>
       </c>
       <c r="K8">
-        <v>0.29352315669215201</v>
+        <v>0.50336338260193103</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -7573,22 +9743,22 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
         <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>138</v>
-      </c>
-      <c r="I9" t="s">
-        <v>134</v>
+        <v>189</v>
+      </c>
+      <c r="I9">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J9">
-        <v>9.7234753064520604E-2</v>
+        <v>0.395844662392418</v>
       </c>
       <c r="K9">
-        <v>0.30248369640627198</v>
+        <v>0.39219958601154797</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -7608,22 +9778,22 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="G10" t="s">
         <v>17</v>
       </c>
       <c r="H10">
-        <v>0.03</v>
+        <v>-0.104</v>
       </c>
       <c r="I10">
-        <v>4.0000000000000001E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="J10">
-        <v>8.3209924303995694E-2</v>
+        <v>0.275303578498655</v>
       </c>
       <c r="K10">
-        <v>0.37324624254340699</v>
+        <v>0.269058295964126</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -7643,22 +9813,22 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="H11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I11" t="s">
-        <v>134</v>
+      <c r="H11">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="I11">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J11">
-        <v>8.3209924303995694E-2</v>
+        <v>0.23764326507414599</v>
       </c>
       <c r="K11">
-        <v>0.37324624254340699</v>
+        <v>0.43520309477756303</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -7678,22 +9848,22 @@
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G12" t="s">
         <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="I12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J12">
-        <v>-3.7465722527858999E-2</v>
+        <v>0.23016734883909001</v>
       </c>
       <c r="K12">
-        <v>6.3627924814454895E-2</v>
+        <v>0.29352315669215201</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -7713,22 +9883,22 @@
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="H13">
-        <v>7.6999999999999999E-2</v>
+      <c r="H13" t="s">
+        <v>189</v>
       </c>
       <c r="I13">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="J13">
-        <v>-8.30165046128611E-2</v>
+        <v>0.20152708546981199</v>
       </c>
       <c r="K13">
-        <v>0.14701478315319499</v>
+        <v>0.39555539573519399</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -7748,22 +9918,22 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="G14" t="s">
         <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>139</v>
-      </c>
-      <c r="I14" t="s">
-        <v>134</v>
+        <v>186</v>
+      </c>
+      <c r="I14">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J14">
-        <v>-8.30165046128611E-2</v>
+        <v>0.19650105360627501</v>
       </c>
       <c r="K14">
-        <v>0.14701478315319499</v>
+        <v>0.433282516248094</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -7783,22 +9953,22 @@
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" t="s">
         <v>17</v>
       </c>
-      <c r="H15" t="s">
-        <v>135</v>
-      </c>
-      <c r="I15" t="s">
-        <v>147</v>
+      <c r="H15">
+        <v>2.4E-2</v>
+      </c>
+      <c r="I15">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J15">
-        <v>-8.7141038638266097E-2</v>
+        <v>0.17582189386248501</v>
       </c>
       <c r="K15">
-        <v>0.31126988535690697</v>
+        <v>0.48155437376994298</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -7818,22 +9988,22 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16" t="s">
         <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I16" t="s">
         <v>134</v>
       </c>
       <c r="J16">
-        <v>-8.9136433339484206E-2</v>
+        <v>9.7234753064520604E-2</v>
       </c>
       <c r="K16">
-        <v>0.22806435561453001</v>
+        <v>0.30248369640627198</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -7853,22 +10023,22 @@
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="G17" t="s">
         <v>17</v>
       </c>
-      <c r="H17" t="s">
-        <v>137</v>
-      </c>
-      <c r="I17" t="s">
-        <v>134</v>
+      <c r="H17">
+        <v>0.03</v>
+      </c>
+      <c r="I17">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J17">
-        <v>-0.120735390600266</v>
+        <v>8.3209924303995694E-2</v>
       </c>
       <c r="K17">
-        <v>6.0377855598125002E-2</v>
+        <v>0.37324624254340699</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -7888,22 +10058,22 @@
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="G18" t="s">
         <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>146</v>
-      </c>
-      <c r="I18" t="s">
-        <v>134</v>
+        <v>185</v>
+      </c>
+      <c r="I18">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J18">
-        <v>-0.14811236431004901</v>
+        <v>6.7778038905043497E-2</v>
       </c>
       <c r="K18">
-        <v>7.8788984132774006E-2</v>
+        <v>0.40709508578074999</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -7923,22 +10093,22 @@
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
         <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>176</v>
-      </c>
-      <c r="I19" t="s">
-        <v>134</v>
+        <v>193</v>
+      </c>
+      <c r="I19">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="J19">
-        <v>-0.14811236431004901</v>
+        <v>-1.6241641763504899E-2</v>
       </c>
       <c r="K19">
-        <v>7.8788984132774006E-2</v>
+        <v>0.37096206439035001</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -7958,22 +10128,22 @@
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G20" t="s">
         <v>17</v>
       </c>
       <c r="H20" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="I20" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="J20">
-        <v>-0.20979362816125499</v>
+        <v>-3.7465722527858999E-2</v>
       </c>
       <c r="K20">
-        <v>0.105383163602571</v>
+        <v>6.3627924814454895E-2</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -7993,22 +10163,22 @@
         <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G21" t="s">
         <v>17</v>
       </c>
       <c r="H21" t="s">
-        <v>136</v>
-      </c>
-      <c r="I21" t="s">
-        <v>134</v>
+        <v>185</v>
+      </c>
+      <c r="I21">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="J21">
-        <v>-0.29361608436110997</v>
+        <v>-6.3778933912280095E-2</v>
       </c>
       <c r="K21">
-        <v>0.12340177561443801</v>
+        <v>0.430938168353178</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -8028,22 +10198,22 @@
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G22" t="s">
         <v>17</v>
       </c>
       <c r="H22">
-        <v>3.5000000000000003E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="I22">
-        <v>5.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J22">
-        <v>-0.32043034098407203</v>
+        <v>-8.30165046128611E-2</v>
       </c>
       <c r="K22">
-        <v>0.41966823078448201</v>
+        <v>0.14701478315319499</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -8063,22 +10233,22 @@
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G23" t="s">
         <v>17</v>
       </c>
       <c r="H23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I23" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="J23">
-        <v>-0.32043034098407203</v>
+        <v>-8.7141038638266097E-2</v>
       </c>
       <c r="K23">
-        <v>0.41966823078448201</v>
+        <v>0.31126988535690697</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -8098,22 +10268,22 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="G24" t="s">
         <v>17</v>
       </c>
-      <c r="H24">
-        <v>-3.5999999999999997E-2</v>
-      </c>
-      <c r="I24">
-        <v>4.0000000000000001E-3</v>
+      <c r="H24" t="s">
+        <v>140</v>
+      </c>
+      <c r="I24" t="s">
+        <v>134</v>
       </c>
       <c r="J24">
-        <v>-0.41431075563352499</v>
+        <v>-8.9136433339484206E-2</v>
       </c>
       <c r="K24">
-        <v>0.309998872731372</v>
+        <v>0.22806435561453001</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -8133,22 +10303,22 @@
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G25" t="s">
         <v>17</v>
       </c>
       <c r="H25" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="I25" t="s">
         <v>134</v>
       </c>
       <c r="J25">
-        <v>-0.42470121872245797</v>
+        <v>-0.120735390600266</v>
       </c>
       <c r="K25">
-        <v>0.43662825955124301</v>
+        <v>6.0377855598125002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -8168,22 +10338,22 @@
         <v>15</v>
       </c>
       <c r="F26" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="G26" t="s">
         <v>17</v>
       </c>
-      <c r="H26">
-        <v>-9.6000000000000002E-2</v>
+      <c r="H26" t="s">
+        <v>191</v>
       </c>
       <c r="I26">
-        <v>1.6E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J26">
-        <v>-0.43834270734766401</v>
+        <v>-0.120997261509139</v>
       </c>
       <c r="K26">
-        <v>0.38691588785046699</v>
+        <v>0.52872752908001397</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -8203,22 +10373,22 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="G27" t="s">
         <v>17</v>
       </c>
-      <c r="H27">
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="I27">
-        <v>4.0000000000000001E-3</v>
+      <c r="H27" t="s">
+        <v>146</v>
+      </c>
+      <c r="I27" t="s">
+        <v>134</v>
       </c>
       <c r="J27">
-        <v>-0.62889153521509</v>
+        <v>-0.14811236431004901</v>
       </c>
       <c r="K27">
-        <v>0.50662686027050297</v>
+        <v>7.8788984132774006E-2</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -8238,22 +10408,22 @@
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G28" t="s">
         <v>17</v>
       </c>
-      <c r="H28" t="s">
-        <v>145</v>
-      </c>
-      <c r="I28" t="s">
-        <v>134</v>
+      <c r="H28">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I28">
+        <v>0.01</v>
       </c>
       <c r="J28">
-        <v>-0.73694337285361899</v>
+        <v>-0.18530099117117799</v>
       </c>
       <c r="K28">
-        <v>0.32188195656097701</v>
+        <v>0.50028793550244699</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -8273,22 +10443,22 @@
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
       <c r="G29" t="s">
         <v>17</v>
       </c>
       <c r="H29">
-        <v>2.3E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="I29">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="J29">
-        <v>-0.84798952666127003</v>
+        <v>-0.185692452647822</v>
       </c>
       <c r="K29">
-        <v>0.431699044094974</v>
+        <v>0.32128750810587797</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -8308,26 +10478,834 @@
         <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G30" t="s">
         <v>17</v>
       </c>
       <c r="H30" t="s">
+        <v>135</v>
+      </c>
+      <c r="I30" t="s">
+        <v>134</v>
+      </c>
+      <c r="J30">
+        <v>-0.20979362816125499</v>
+      </c>
+      <c r="K30">
+        <v>0.105383163602571</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>297</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>127</v>
+      </c>
+      <c r="G31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="I31">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J31">
+        <v>-0.22385287731784101</v>
+      </c>
+      <c r="K31">
+        <v>0.28436902708498402</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>298</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="s">
+        <v>189</v>
+      </c>
+      <c r="I32">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J32">
+        <v>-0.28673559390332198</v>
+      </c>
+      <c r="K32">
+        <v>0.38341634715304401</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>299</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" t="s">
+        <v>136</v>
+      </c>
+      <c r="I33" t="s">
+        <v>134</v>
+      </c>
+      <c r="J33">
+        <v>-0.29361608436110997</v>
+      </c>
+      <c r="K33">
+        <v>0.12340177561443801</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>300</v>
+      </c>
+      <c r="D34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" t="s">
+        <v>112</v>
+      </c>
+      <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" t="s">
+        <v>187</v>
+      </c>
+      <c r="I34">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J34">
+        <v>-0.298055121920277</v>
+      </c>
+      <c r="K34">
+        <v>0.48237151376951398</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>301</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I35">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J35">
+        <v>-0.32043034098407203</v>
+      </c>
+      <c r="K35">
+        <v>0.41966823078448201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>302</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>124</v>
+      </c>
+      <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" t="s">
+        <v>190</v>
+      </c>
+      <c r="I36">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J36">
+        <v>-0.35304644548957498</v>
+      </c>
+      <c r="K36">
+        <v>0.40752465160280898</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>303</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I37">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J37">
+        <v>-0.36616018228963698</v>
+      </c>
+      <c r="K37">
+        <v>0.457707799340901</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>304</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I38">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J38">
+        <v>-0.41431075563352499</v>
+      </c>
+      <c r="K38">
+        <v>0.309998872731372</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>305</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" t="s">
+        <v>74</v>
+      </c>
+      <c r="G39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" t="s">
+        <v>148</v>
+      </c>
+      <c r="I39" t="s">
+        <v>134</v>
+      </c>
+      <c r="J39">
+        <v>-0.42470121872245797</v>
+      </c>
+      <c r="K39">
+        <v>0.43662825955124301</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" t="s">
+        <v>306</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I40">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J40">
+        <v>-0.43493149949916099</v>
+      </c>
+      <c r="K40">
+        <v>0.48497484476272501</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>307</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>54</v>
+      </c>
+      <c r="G41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41">
+        <v>-9.6000000000000002E-2</v>
+      </c>
+      <c r="I41">
+        <v>1.6E-2</v>
+      </c>
+      <c r="J41">
+        <v>-0.43834270734766401</v>
+      </c>
+      <c r="K41">
+        <v>0.38691588785046699</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" t="s">
+        <v>308</v>
+      </c>
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" t="s">
+        <v>114</v>
+      </c>
+      <c r="G42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I42">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J42">
+        <v>-0.46565820135735098</v>
+      </c>
+      <c r="K42">
+        <v>0.51735490546514895</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" t="s">
+        <v>309</v>
+      </c>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>121</v>
+      </c>
+      <c r="G43" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" t="s">
+        <v>192</v>
+      </c>
+      <c r="I43">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J43">
+        <v>-0.50507817642654196</v>
+      </c>
+      <c r="K43">
+        <v>0.49167756777482102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>310</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>113</v>
+      </c>
+      <c r="G44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" t="s">
+        <v>188</v>
+      </c>
+      <c r="I44">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J44">
+        <v>-0.54393212711267602</v>
+      </c>
+      <c r="K44">
+        <v>0.44209702660406902</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>311</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="I45">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J45">
+        <v>-0.62889153521509</v>
+      </c>
+      <c r="K45">
+        <v>0.50662686027050297</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" t="s">
+        <v>312</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46">
+        <v>2.3E-2</v>
+      </c>
+      <c r="I46">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J46">
+        <v>-0.68361041975036396</v>
+      </c>
+      <c r="K46">
+        <v>0.48074802628677299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" t="s">
+        <v>313</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" t="s">
+        <v>145</v>
+      </c>
+      <c r="I47" t="s">
+        <v>134</v>
+      </c>
+      <c r="J47">
+        <v>-0.73694337285361899</v>
+      </c>
+      <c r="K47">
+        <v>0.32188195656097701</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>314</v>
+      </c>
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" t="s">
+        <v>188</v>
+      </c>
+      <c r="I48">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J48">
+        <v>-0.84798952666127003</v>
+      </c>
+      <c r="K48">
+        <v>0.431699044094974</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" t="s">
+        <v>315</v>
+      </c>
+      <c r="D49" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" t="s">
+        <v>123</v>
+      </c>
+      <c r="G49" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49">
+        <v>0.02</v>
+      </c>
+      <c r="I49">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J49">
+        <v>-0.85433760262868597</v>
+      </c>
+      <c r="K49">
+        <v>0.53973013493253397</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" t="s">
+        <v>316</v>
+      </c>
+      <c r="D50" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" t="s">
+        <v>126</v>
+      </c>
+      <c r="G50" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" t="s">
+        <v>187</v>
+      </c>
+      <c r="I50">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J50">
+        <v>-1.0825650582392301</v>
+      </c>
+      <c r="K50">
+        <v>0.485788554139856</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" t="s">
+        <v>317</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" t="s">
+        <v>72</v>
+      </c>
+      <c r="G51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" t="s">
         <v>143</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I51" t="s">
         <v>144</v>
       </c>
-      <c r="J30">
+      <c r="J51">
         <v>-1.2550855746723999</v>
       </c>
-      <c r="K30">
+      <c r="K51">
         <v>0.28880866425992802</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" t="s">
+        <v>109</v>
+      </c>
+      <c r="G52" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I52">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J52">
+        <v>-1.3374852552877901</v>
+      </c>
+      <c r="K52">
+        <v>0.46993613688396202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" t="s">
+        <v>319</v>
+      </c>
+      <c r="D53" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" t="s">
+        <v>115</v>
+      </c>
+      <c r="G53" t="s">
+        <v>17</v>
+      </c>
+      <c r="H53" t="s">
+        <v>190</v>
+      </c>
+      <c r="I53">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J53">
+        <v>-1.38337156657076</v>
+      </c>
+      <c r="K53">
+        <v>0.39098520895577399</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
+  <conditionalFormatting sqref="F2:F53">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>